<commit_message>
Finishing Legacy sec regression and cutover procs
</commit_message>
<xml_diff>
--- a/doc/regression-test/suites/legacy-security/01-basic.xlsx
+++ b/doc/regression-test/suites/legacy-security/01-basic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\Dev\Propel\propel\doc\regression-test\suites\legacy-security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCECAFCD-F306-49E8-B4F6-B8F555E96A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63944E84-5006-4F50-BD3A-9FD8D9C66523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="162">
   <si>
     <t>Description</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Not Executed</t>
-  </si>
-  <si>
     <t>Step Details</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>The "Executions in last 30 days" chart is displayed</t>
   </si>
   <si>
-    <t>The login option in the User menu is hidden.</t>
-  </si>
-  <si>
     <t>Click in the Back to home button in the upper left corner of the navigation bar</t>
   </si>
   <si>
@@ -208,15 +202,9 @@
     <t>Check if all the expected cards are being displayed.</t>
   </si>
   <si>
-    <t>Login option</t>
-  </si>
-  <si>
     <t>Validate a "blue" User icon is displayed as corresponding when Legacy Security is enabled.</t>
   </si>
   <si>
-    <t>Check links in Navbar: Quick Task, Worflows, Scripts Targets and History links.</t>
-  </si>
-  <si>
     <t>All are present</t>
   </si>
   <si>
@@ -238,15 +226,9 @@
     <t>Enter any text in the Search text area in the navigation bar</t>
   </si>
   <si>
-    <t>Click on the Add a Target button in the Get Started section</t>
-  </si>
-  <si>
     <t>The new target form is displayed</t>
   </si>
   <si>
-    <t>Fill the required fields and click on the save button</t>
-  </si>
-  <si>
     <t>A "Changes have been saved successfully" toast is displayed.</t>
   </si>
   <si>
@@ -293,9 +275,6 @@
   </si>
   <si>
     <t>Click in the go back botton at top left in the nav bar.</t>
-  </si>
-  <si>
-    <t>Click on the Upload your Script button in the Get Started section</t>
   </si>
   <si>
     <t>An empty form for a new Script is displayed. In the form you can see 3 tabs, (Details, Code and Finish). The active tab is Details</t>
@@ -397,34 +376,16 @@
     <t>03_Scripts</t>
   </si>
   <si>
-    <t>User menu is working and displaying the right options.</t>
-  </si>
-  <si>
-    <t>User menu expand and collapse and is displaying the options to create/manage credentials as also to create/manage Users.</t>
-  </si>
-  <si>
     <t>The following cards must be displayed: Get Started, Lastest activities, Most popular workflows, Last errors.
 The card My Favorite Workflows is not displayed for legacy security, (Unknown user)</t>
   </si>
   <si>
-    <t>The log off option in the User menu is hidden.</t>
-  </si>
-  <si>
-    <t>Log off option</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
     <t>Move to next button is now enabled</t>
   </si>
   <si>
-    <t>/doc/test-scripts/test-remote.ps1</t>
-  </si>
-  <si>
-    <t>Links and User menu</t>
-  </si>
-  <si>
     <t>Page Content</t>
   </si>
   <si>
@@ -447,9 +408,6 @@
   </si>
   <si>
     <t>Add a Script</t>
-  </si>
-  <si>
-    <t>Add another functionality</t>
   </si>
   <si>
     <t>Browse scripts</t>
@@ -545,6 +503,89 @@
   </si>
   <si>
     <t>You are redirected to Home page and all the changes are lost.</t>
+  </si>
+  <si>
+    <t>\doc\test-scripts\test-remote.ps1</t>
+  </si>
+  <si>
+    <t>Check links in Navbar: Quick Task, Worflows, Scripts Targets, History and More links.</t>
+  </si>
+  <si>
+    <t>Check "User" menu</t>
+  </si>
+  <si>
+    <t>Check "More" menu</t>
+  </si>
+  <si>
+    <t>the More menu expand and collapse and is displaying:
+Basic options to Add targets, upload scripts and Create Workflows. Also to create the 3 types of Credentials: Win, AWS and API.
+Create User and manage both Users and Credentials.</t>
+  </si>
+  <si>
+    <t>Navigation bar</t>
+  </si>
+  <si>
+    <t>User menu expand and collapse and is displaying only the Login option.</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Add a Target" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Upload your script" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Ctreate a Workflow" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New Windows Credential" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New Amazon Web Services Credential" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New Generic API Key Creential" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New User Account" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Manage Credentials" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Manage Users" option</t>
+  </si>
+  <si>
+    <t>You are redirected to a new Windows credential form.</t>
+  </si>
+  <si>
+    <t>You are redirected to a new AWS credential form.</t>
+  </si>
+  <si>
+    <t>You are redirected to a new API credential form.</t>
+  </si>
+  <si>
+    <t>You are redirected to a new user page</t>
+  </si>
+  <si>
+    <t>You are redirected to the browse credentials page</t>
+  </si>
+  <si>
+    <t>You are redirected to the Browse users page</t>
+  </si>
+  <si>
+    <t>Click on the "More" menu to expand it and then in the Add a Target option.</t>
+  </si>
+  <si>
+    <t>Fill only the required fields and click on the save button</t>
+  </si>
+  <si>
+    <t>Click on the Upload your Script option from the More menu.</t>
+  </si>
+  <si>
+    <t>Add another</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
   </si>
 </sst>
 </file>
@@ -838,7 +879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -897,6 +938,18 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -912,48 +965,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="86">
     <dxf>
       <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -975,8 +997,12 @@
       <font>
         <b/>
         <i val="0"/>
-        <strike val="0"/>
-      </font>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -996,24 +1022,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1028,6 +1036,13 @@
           <bgColor rgb="FFF1826F"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1049,8 +1064,12 @@
       <font>
         <b/>
         <i val="0"/>
-        <strike val="0"/>
-      </font>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1062,385 +1081,6 @@
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1782,6 +1422,153 @@
       <font>
         <b val="0"/>
         <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
@@ -2405,6 +2192,247 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3582,11 +3610,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}" name="Summary" displayName="Summary" ref="A1:B4" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}" name="Summary" displayName="Summary" ref="A1:B4" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83" totalsRowBorderDxfId="82">
   <autoFilter ref="A1:B4" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{654C6343-7B3C-42FE-9EF4-7BFE7BE35779}" name="Test Case Sheet name" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{FDA0E746-B4F2-405E-8A1D-9A6A22073CB9}" name="Result" dataDxfId="87">
+    <tableColumn id="1" xr3:uid="{654C6343-7B3C-42FE-9EF4-7BFE7BE35779}" name="Test Case Sheet name" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{FDA0E746-B4F2-405E-8A1D-9A6A22073CB9}" name="Result" dataDxfId="80">
       <calculatedColumnFormula array="1">INDIRECT(A2&amp;"!E8")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3595,22 +3623,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}" name="SummaryResults" displayName="SummaryResults" ref="D1:E4" totalsRowShown="0" headerRowDxfId="86" headerRowBorderDxfId="85" tableBorderDxfId="84" totalsRowBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}" name="SummaryResults" displayName="SummaryResults" ref="D1:E4" totalsRowShown="0" headerRowDxfId="79" headerRowBorderDxfId="78" tableBorderDxfId="77" totalsRowBorderDxfId="76">
   <autoFilter ref="D1:E4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5420B28C-70A3-47FD-BF8A-F016E4F7FA0F}" name="Summary Results" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{B0E66881-1E02-43BC-AA03-3C33769D1162}" name="Count" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{5420B28C-70A3-47FD-BF8A-F016E4F7FA0F}" name="Summary Results" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{B0E66881-1E02-43BC-AA03-3C33769D1162}" name="Count" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C89B2B93-96BB-441E-B77B-7E40B50E056D}" name="SampleTestCase12" displayName="SampleTestCase12" ref="A10:F27" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79" tableBorderDxfId="77" totalsRowBorderDxfId="76">
-  <autoFilter ref="A10:F27" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C89B2B93-96BB-441E-B77B-7E40B50E056D}" name="SampleTestCase12" displayName="SampleTestCase12" ref="A10:F35" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="A10:F35" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3619,21 +3647,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{07F3C726-CF4B-4A89-9D4E-FFC2F3B71504}" name="Step#" dataDxfId="75">
+    <tableColumn id="1" xr3:uid="{07F3C726-CF4B-4A89-9D4E-FFC2F3B71504}" name="Step#" dataDxfId="50">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3B181203-88B8-4ECA-8586-E1A7969EA7C0}" name="Area" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{302EA2CC-144C-447A-9537-518BDA10AB76}" name="Step Details" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{9F997859-00F8-4561-BA64-59F450F04E06}" name="Expected" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{CAFD8264-06FC-4330-A577-54F901209313}" name="Actual" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{16774486-6CCF-4804-BFB8-5A09A9868319}" name="Status" dataDxfId="70"/>
+    <tableColumn id="6" xr3:uid="{3B181203-88B8-4ECA-8586-E1A7969EA7C0}" name="Area" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{302EA2CC-144C-447A-9537-518BDA10AB76}" name="Step Details" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{9F997859-00F8-4561-BA64-59F450F04E06}" name="Expected" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{CAFD8264-06FC-4330-A577-54F901209313}" name="Actual" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{16774486-6CCF-4804-BFB8-5A09A9868319}" name="Status" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3B579B8E-71E0-43F3-BD7B-444793913C5A}" name="SampleTestCase123" displayName="SampleTestCase123" ref="A10:F21" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68" tableBorderDxfId="66" totalsRowBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3B579B8E-71E0-43F3-BD7B-444793913C5A}" name="SampleTestCase123" displayName="SampleTestCase123" ref="A10:F21" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="A10:F21" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3643,21 +3671,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0AA68334-D062-478E-B0C8-2A2CFFD191F2}" name="Step#" dataDxfId="64">
+    <tableColumn id="1" xr3:uid="{0AA68334-D062-478E-B0C8-2A2CFFD191F2}" name="Step#" dataDxfId="39">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6AA83282-0CB1-43FB-B377-DD7C842943BA}" name="Area" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{1BC430D2-4E88-4EB3-A940-5C76D8B44147}" name="Step Details" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{A9EC0C70-AC5B-4C7B-9581-F62CC5CABAE0}" name="Expected" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{65718CE7-73C9-43E5-BEB5-4042B4E01F30}" name="Actual" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{F0DA7687-947E-491E-B21A-6C6F2A460B02}" name="Status" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{6AA83282-0CB1-43FB-B377-DD7C842943BA}" name="Area" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{1BC430D2-4E88-4EB3-A940-5C76D8B44147}" name="Step Details" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{A9EC0C70-AC5B-4C7B-9581-F62CC5CABAE0}" name="Expected" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{65718CE7-73C9-43E5-BEB5-4042B4E01F30}" name="Actual" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{F0DA7687-947E-491E-B21A-6C6F2A460B02}" name="Status" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2E377BD4-3235-49A1-8093-E3126E000F02}" name="SampleTestCase1236" displayName="SampleTestCase1236" ref="A10:F39" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2E377BD4-3235-49A1-8093-E3126E000F02}" name="SampleTestCase1236" displayName="SampleTestCase1236" ref="A10:F39" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="A10:F39" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3667,14 +3695,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D212E0A2-335D-478C-B756-642813E0558C}" name="Step#" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{D212E0A2-335D-478C-B756-642813E0558C}" name="Step#" dataDxfId="17">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16DCD7B5-32CF-48ED-AED3-35BA513DBB2D}" name="Area" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{AEE0C5E2-2C55-481B-8027-6186153E70AE}" name="Step Details" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{282D8BD2-B088-4502-A54F-900ED78CEE98}" name="Expected" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{EFCD6DDD-E11D-47C7-B40B-FC360F320FD4}" name="Actual" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{50EF06F8-03DD-4928-922F-2B85123D772A}" name="Status" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{16DCD7B5-32CF-48ED-AED3-35BA513DBB2D}" name="Area" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{AEE0C5E2-2C55-481B-8027-6186153E70AE}" name="Step Details" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{282D8BD2-B088-4502-A54F-900ED78CEE98}" name="Expected" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{EFCD6DDD-E11D-47C7-B40B-FC360F320FD4}" name="Actual" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{50EF06F8-03DD-4928-922F-2B85123D772A}" name="Status" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3945,8 +3973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1510635-E20C-4AD1-9756-3BB17945F573}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3960,28 +3988,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">INDIRECT(A2&amp;"!E8")</f>
         <v>Not Executed</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5">
         <f ca="1">COUNTIF(Summary[Result],"Not Executed")</f>
@@ -3990,14 +4018,14 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B3" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">INDIRECT(A3&amp;"!E8")</f>
         <v>Not Executed</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5">
         <f ca="1">COUNTIF(Summary[Result],"Pass")</f>
@@ -4006,14 +4034,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B4" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B4" ca="1">INDIRECT(A4&amp;"!E8")</f>
         <v>Not Executed</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">COUNTIF(Summary[Result],"Fail")</f>
@@ -4034,10 +4062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59558529-F109-4122-99C6-22F7311C314B}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4059,14 +4087,14 @@
       <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4076,21 +4104,21 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5">
         <f>COUNTIF(SampleTestCase12[Status], "Not Executed")</f>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F5" s="15">
         <f>E5/SUM(E$5:E$7)</f>
@@ -4099,10 +4127,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5">
         <f>COUNTIF(SampleTestCase12[Status], "Pass")</f>
@@ -4115,10 +4143,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5">
         <f>COUNTIF(SampleTestCase12[Status], "Fail")</f>
@@ -4131,17 +4159,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="24" t="str">
+        <v>7</v>
+      </c>
+      <c r="E8" s="28" t="str">
         <f>IF(E7&gt;0, "Fail",
     IF(E5&gt;0, "Not Executed", "Pass"))</f>
         <v>Not Executed</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -4149,10 +4177,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>3</v>
@@ -4166,21 +4194,21 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <f t="shared" ref="A11:A27" si="1">IF(ISNUMBER(A10), A10 +1, 1)</f>
+        <f t="shared" ref="A11:A35" si="1">IF(ISNUMBER(A10), A10 +1, 1)</f>
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4189,17 +4217,17 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4208,112 +4236,112 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="91" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
       <c r="B16" s="10" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="65" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="65" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>39</v>
+        <v>98</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="E18" s="17"/>
       <c r="F18" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4322,17 +4350,17 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4341,7 +4369,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>26</v>
@@ -4351,7 +4379,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4360,7 +4388,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>28</v>
@@ -4370,7 +4398,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4379,7 +4407,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>30</v>
@@ -4389,7 +4417,7 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4398,7 +4426,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>32</v>
@@ -4408,7 +4436,7 @@
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4417,55 +4445,55 @@
         <v>14</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>45</v>
+        <v>98</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4474,17 +4502,169 @@
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>49</v>
+        <v>98</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>143</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A29" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A30" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A33" s="5">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A34" s="5">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4496,34 +4676,94 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F27">
-    <cfRule type="expression" dxfId="39" priority="1">
+  <conditionalFormatting sqref="F11:F35">
+    <cfRule type="expression" dxfId="73" priority="3">
       <formula>$F11="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="2">
+    <cfRule type="expression" dxfId="72" priority="4">
       <formula>$F11="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="37" priority="3">
+    <cfRule type="expression" dxfId="71" priority="5">
       <formula>$E$8="Pass"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="4">
+    <cfRule type="expression" dxfId="70" priority="6">
       <formula>$E$8="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:F27">
-    <cfRule type="expression" dxfId="35" priority="6">
+  <conditionalFormatting sqref="A11:E11 B26:B33 C27:C33 B12:E25 A12:A35 C26:E26">
+    <cfRule type="expression" dxfId="69" priority="8">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B27">
-    <cfRule type="expression" dxfId="34" priority="5">
+  <conditionalFormatting sqref="B11:B33">
+    <cfRule type="expression" dxfId="68" priority="7">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B35:E35">
+    <cfRule type="expression" dxfId="67" priority="20">
+      <formula>AND($B35&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="66" priority="22">
+      <formula>AND($B35&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:E34">
+    <cfRule type="expression" dxfId="65" priority="24">
+      <formula>AND($B34&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:E33">
+    <cfRule type="expression" dxfId="64" priority="28">
+      <formula>AND($B32&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="expression" dxfId="63" priority="32">
+      <formula>AND($B31&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="expression" dxfId="62" priority="36">
+      <formula>AND($B30&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="expression" dxfId="61" priority="40">
+      <formula>AND($B29&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="expression" dxfId="60" priority="44">
+      <formula>AND($B28&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27 B34:C34">
+    <cfRule type="expression" dxfId="59" priority="48">
+      <formula>AND($B27&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="58" priority="54">
+      <formula>AND($B34&lt;&gt;$B32)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D28">
+    <cfRule type="expression" dxfId="57" priority="2">
+      <formula>AND($B27&lt;&gt;$B26)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D31">
+    <cfRule type="expression" dxfId="56" priority="1">
+      <formula>AND($B29&lt;&gt;$B28)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F27" xr:uid="{1795B932-808D-4E1C-B6CC-3657CE692FEA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F35" xr:uid="{1795B932-808D-4E1C-B6CC-3657CE692FEA}">
       <formula1>"Pass,Fail,Not Executed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4539,8 +4779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EC76D5-508E-49A8-8CA4-8BD5DC983C38}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4562,14 +4802,14 @@
       <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4579,17 +4819,17 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5">
         <f>COUNTIF(SampleTestCase123[Status], "Not Executed")</f>
@@ -4602,10 +4842,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5">
         <f>COUNTIF(SampleTestCase123[Status], "Pass")</f>
@@ -4618,10 +4858,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5">
         <f>COUNTIF(SampleTestCase123[Status], "Fail")</f>
@@ -4634,17 +4874,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="24" t="str">
+        <v>7</v>
+      </c>
+      <c r="E8" s="28" t="str">
         <f>IF(E7&gt;0, "Fail",
     IF(E5&gt;0, "Not Executed", "Pass"))</f>
         <v>Not Executed</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -4652,10 +4892,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>3</v>
@@ -4673,17 +4913,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4692,17 +4932,17 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4711,17 +4951,17 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4730,17 +4970,17 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4749,17 +4989,17 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4768,17 +5008,17 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4787,17 +5027,17 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4806,17 +5046,17 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4825,17 +5065,17 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4844,17 +5084,17 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4863,17 +5103,17 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4886,28 +5126,28 @@
     <mergeCell ref="E8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F21">
-    <cfRule type="expression" dxfId="33" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>$F11="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>$F11="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="31" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>$E$8="Pass"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$E$8="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:F21">
-    <cfRule type="expression" dxfId="29" priority="6">
+  <conditionalFormatting sqref="A11:E21">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B21">
-    <cfRule type="expression" dxfId="28" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4928,8 +5168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0284662-B42C-4A0F-B1ED-3CE18BC81596}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4951,14 +5191,14 @@
       <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4968,21 +5208,21 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="B5" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="26"/>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5">
         <f>COUNTIF(SampleTestCase1236[Status], "Not Executed")</f>
@@ -4995,14 +5235,14 @@
     </row>
     <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="22"/>
+        <v>115</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="26"/>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5">
         <f>COUNTIF(SampleTestCase1236[Status], "Pass")</f>
@@ -5015,14 +5255,14 @@
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="22"/>
+        <v>117</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="26"/>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5">
         <f>COUNTIF(SampleTestCase1236[Status], "Fail")</f>
@@ -5035,21 +5275,21 @@
     </row>
     <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="22"/>
+        <v>118</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="26"/>
       <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="24" t="str">
+        <v>7</v>
+      </c>
+      <c r="E8" s="28" t="str">
         <f>IF(E7&gt;0, "Fail",
     IF(E5&gt;0, "Not Executed", "Pass"))</f>
         <v>Not Executed</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -5057,10 +5297,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>3</v>
@@ -5078,17 +5318,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5097,17 +5337,17 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5116,17 +5356,17 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5135,17 +5375,17 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5154,17 +5394,17 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5173,17 +5413,17 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5192,17 +5432,17 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5211,17 +5451,17 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5230,17 +5470,17 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5249,17 +5489,17 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5268,17 +5508,17 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -5287,17 +5527,17 @@
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5306,17 +5546,17 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5325,17 +5565,17 @@
         <v>14</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5344,17 +5584,17 @@
         <v>15</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5363,17 +5603,17 @@
         <v>16</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5382,17 +5622,17 @@
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5401,17 +5641,17 @@
         <v>18</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5420,17 +5660,17 @@
         <v>19</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5439,17 +5679,17 @@
         <v>20</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5458,17 +5698,17 @@
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="27"/>
+        <v>111</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="23"/>
       <c r="F31" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5477,17 +5717,17 @@
         <v>22</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5496,17 +5736,17 @@
         <v>23</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5515,17 +5755,17 @@
         <v>24</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>111</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="23"/>
       <c r="F34" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5534,17 +5774,17 @@
         <v>25</v>
       </c>
       <c r="B35" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" s="27"/>
+      <c r="D35" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="23"/>
       <c r="F35" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5553,17 +5793,17 @@
         <v>26</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="27"/>
+        <v>127</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="23"/>
       <c r="F36" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5572,17 +5812,17 @@
         <v>27</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" s="27"/>
+        <v>127</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="23"/>
       <c r="F37" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5591,17 +5831,17 @@
         <v>28</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E38" s="27"/>
+        <v>127</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="23"/>
       <c r="F38" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5610,17 +5850,17 @@
         <v>29</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="E39" s="27"/>
+        <v>127</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="23"/>
       <c r="F39" s="4" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -5633,53 +5873,53 @@
     <mergeCell ref="E8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F39">
-    <cfRule type="expression" dxfId="27" priority="5">
+    <cfRule type="expression" dxfId="33" priority="5">
       <formula>$F11="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="6">
+    <cfRule type="expression" dxfId="32" priority="6">
       <formula>$F11="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="25" priority="7">
+    <cfRule type="expression" dxfId="31" priority="7">
       <formula>$E$8="Pass"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>$E$8="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:F11 C32:F32 F31:F35 B12:F31 B31:B35 B37:B39 B36:F36 A12:A39">
-    <cfRule type="expression" dxfId="23" priority="10">
+  <conditionalFormatting sqref="A11:F11 C32:F32 B31:B35 B37:B39 B36:F36 A12:A39 B12:F31 F12:F39">
+    <cfRule type="expression" dxfId="29" priority="10">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B39">
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="28" priority="9">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:F33">
-    <cfRule type="expression" dxfId="21" priority="16">
+    <cfRule type="expression" dxfId="27" priority="16">
       <formula>AND($B33&lt;&gt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:D34">
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>AND($B34&lt;&gt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:D35">
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="25" priority="3">
       <formula>AND($B35&lt;&gt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:F39">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>AND($B37&lt;&gt;$B36)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>AND($B38&lt;&gt;$B37)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Configuration and regression test changes
</commit_message>
<xml_diff>
--- a/doc/regression-test/suites/legacy-security/01-basic.xlsx
+++ b/doc/regression-test/suites/legacy-security/01-basic.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\Dev\Propel\propel\doc\regression-test\suites\legacy-security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63944E84-5006-4F50-BD3A-9FD8D9C66523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912F5483-C330-4E9B-8D6F-D6DF96F19684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="01_Basics" sheetId="13" r:id="rId2"/>
     <sheet name="02_Targets" sheetId="14" r:id="rId3"/>
     <sheet name="03_Scripts" sheetId="15" r:id="rId4"/>
+    <sheet name="04_Users" sheetId="16" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="207">
   <si>
     <t>Description</t>
   </si>
@@ -511,81 +512,225 @@
     <t>Check links in Navbar: Quick Task, Worflows, Scripts Targets, History and More links.</t>
   </si>
   <si>
-    <t>Check "User" menu</t>
-  </si>
-  <si>
     <t>Check "More" menu</t>
   </si>
   <si>
+    <t>Navigation bar</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Add a Target" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Upload your script" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Ctreate a Workflow" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New Windows Credential" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New Amazon Web Services Credential" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New Generic API Key Creential" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "New User Account" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Manage Credentials" option</t>
+  </si>
+  <si>
+    <t>Click in the More menu link in the nav bar. Then click the "Manage Users" option</t>
+  </si>
+  <si>
+    <t>You are redirected to a new Windows credential form.</t>
+  </si>
+  <si>
+    <t>You are redirected to a new AWS credential form.</t>
+  </si>
+  <si>
+    <t>You are redirected to a new API credential form.</t>
+  </si>
+  <si>
+    <t>You are redirected to a new user page</t>
+  </si>
+  <si>
+    <t>You are redirected to the browse credentials page</t>
+  </si>
+  <si>
+    <t>You are redirected to the Browse users page</t>
+  </si>
+  <si>
+    <t>Click on the "More" menu to expand it and then in the Add a Target option.</t>
+  </si>
+  <si>
+    <t>Fill only the required fields and click on the save button</t>
+  </si>
+  <si>
+    <t>Click on the Upload your Script option from the More menu.</t>
+  </si>
+  <si>
+    <t>Add another</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
+  <si>
     <t>the More menu expand and collapse and is displaying:
-Basic options to Add targets, upload scripts and Create Workflows. Also to create the 3 types of Credentials: Win, AWS and API.
+Basic options to Add targets, upload scripts and Create Workflows. Also to create the 4 types of Credentials: Win, AWS, DB and API.
 Create User and manage both Users and Credentials.</t>
   </si>
   <si>
-    <t>Navigation bar</t>
-  </si>
-  <si>
-    <t>User menu expand and collapse and is displaying only the Login option.</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "Add a Target" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "Upload your script" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "Ctreate a Workflow" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "New Windows Credential" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "New Amazon Web Services Credential" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "New Generic API Key Creential" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "New User Account" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "Manage Credentials" option</t>
-  </si>
-  <si>
-    <t>Click in the More menu link in the nav bar. Then click the "Manage Users" option</t>
-  </si>
-  <si>
-    <t>You are redirected to a new Windows credential form.</t>
-  </si>
-  <si>
-    <t>You are redirected to a new AWS credential form.</t>
-  </si>
-  <si>
-    <t>You are redirected to a new API credential form.</t>
-  </si>
-  <si>
-    <t>You are redirected to a new user page</t>
-  </si>
-  <si>
-    <t>You are redirected to the browse credentials page</t>
-  </si>
-  <si>
-    <t>You are redirected to the Browse users page</t>
-  </si>
-  <si>
-    <t>Click on the "More" menu to expand it and then in the Add a Target option.</t>
-  </si>
-  <si>
-    <t>Fill only the required fields and click on the save button</t>
-  </si>
-  <si>
-    <t>Click on the Upload your Script option from the More menu.</t>
-  </si>
-  <si>
-    <t>Add another</t>
-  </si>
-  <si>
-    <t>Not Executed</t>
+    <t>Click in the More menu link in the nav bar. Then click the "New Database Creential" option</t>
+  </si>
+  <si>
+    <t>You are redirected to a new Database credential form.</t>
+  </si>
+  <si>
+    <t>04_Users</t>
+  </si>
+  <si>
+    <t>Testing users CRUD functionality and Validations.</t>
+  </si>
+  <si>
+    <t>Delete "propel.user"</t>
+  </si>
+  <si>
+    <t>A legend saying "This information is required in order to continue." is present below each field but not for the field "Role"</t>
+  </si>
+  <si>
+    <t>First click over each one of the fields, you must see a legend indicating that field is required with exception of Role</t>
+  </si>
+  <si>
+    <t>You see the legend "This can't be longer than 25. (Need to remove at least xxxx chars)</t>
+  </si>
+  <si>
+    <t>Type a long user name of more than 25 chars</t>
+  </si>
+  <si>
+    <t>Type a long display name of more than 50 chars</t>
+  </si>
+  <si>
+    <t>Type in the "initials" field more than 2 chars.</t>
+  </si>
+  <si>
+    <t>Add an invalid email address.</t>
+  </si>
+  <si>
+    <t>You must see the legend "The user e-mail must be a valid email".</t>
+  </si>
+  <si>
+    <t>Open user page</t>
+  </si>
+  <si>
+    <t>User form validations</t>
+  </si>
+  <si>
+    <t>Again in the user name field type anything different than a letter, a number or a dot character</t>
+  </si>
+  <si>
+    <t>You must see the legend "The user name can contain letters, numbers and the dot character only."</t>
+  </si>
+  <si>
+    <t>You must see the legend "This can't be longer than 50. (Need to remove at least xxxx chars)"</t>
+  </si>
+  <si>
+    <t>You must see the legend "This can't be longer than 2. (Need to remove at least xxxx chars)"</t>
+  </si>
+  <si>
+    <t>Type in the "initials" field a number or symbol,(anything different than a letter).</t>
+  </si>
+  <si>
+    <t>You must see the legend "The user initials can contain only letters.".</t>
+  </si>
+  <si>
+    <t>Add a user</t>
+  </si>
+  <si>
+    <t>.Fill the form with the following values:
+User name: propel.user
+Display name: Propel User
+Initials: PU
+e-mail: propel.user@propel.com
+Role User
+Click in the save button</t>
+  </si>
+  <si>
+    <t>Revert changes</t>
+  </si>
+  <si>
+    <t>You will se a toast indicating the changes have been saved successfully.
+Also, "cancel" button is now disabled.</t>
+  </si>
+  <si>
+    <t>Now update all fields for another valid set of values.</t>
+  </si>
+  <si>
+    <t>Now the "Cancel" button is back enabled.</t>
+  </si>
+  <si>
+    <t>Click in the "Cancel" button</t>
+  </si>
+  <si>
+    <t>All the changes are reverted and now the fields had the exact data as when they were saved.</t>
+  </si>
+  <si>
+    <t>Manage Users</t>
+  </si>
+  <si>
+    <t>Click on the "More" user menu and the select the "Manage Users" option</t>
+  </si>
+  <si>
+    <t>The list of users is displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You must see a tooltip that is displaying the creation/update dates and indicate the user never log in. </t>
+  </si>
+  <si>
+    <t>Locate the "Propel User" user and hover the mouse in his initials ("PU") or the Display name.</t>
+  </si>
+  <si>
+    <t>Locking the user</t>
+  </si>
+  <si>
+    <t>Click the lock button at the right of the display name.
+Then confirm in the dialog by clicking the "Ok" button.</t>
+  </si>
+  <si>
+    <t>The user is now locked and the button change his legend to "Unlock"</t>
+  </si>
+  <si>
+    <t>Editing the user</t>
+  </si>
+  <si>
+    <t>Click in the User display name.</t>
+  </si>
+  <si>
+    <t>You must see now the form to edit the user.</t>
+  </si>
+  <si>
+    <t>Chnage the user name as "propel.user.2" and click the "Save" button.</t>
+  </si>
+  <si>
+    <t>Navigate again to the "Manage Users" page and check the changes.</t>
+  </si>
+  <si>
+    <t>The updated user name is displayed in the list of users for "Propel User".</t>
+  </si>
+  <si>
+    <t>Ensure the user with name "propel.user" doesn't exists in the database before to start.</t>
+  </si>
+  <si>
+    <t>Click on the "More" user menu and then select the "New User Account" option</t>
+  </si>
+  <si>
+    <t>A form to add a new user showing the fields: User name, Display name, Initials, email and Role is displayed</t>
+  </si>
+  <si>
+    <t>You will see a toast indicating the changes have been saved successfully.
+Also, "cancel" button is now disabled.</t>
   </si>
 </sst>
 </file>
@@ -879,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -935,12 +1080,6 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -969,7 +1108,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="98">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -995,57 +1178,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <color auto="1"/>
@@ -1067,6 +1199,28 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFF1826F"/>
         </patternFill>
       </fill>
@@ -1084,6 +1238,93 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -1103,6 +1344,299 @@
           <bgColor rgb="FFF1826F"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1422,153 +1956,6 @@
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
@@ -2122,19 +2509,76 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color rgb="FFA6A6A6"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color rgb="FFA6A6A6"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color rgb="FFA6A6A6"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFEDEDED"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FFBFBFBF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF31849B"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2153,6 +2597,263 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBCBCBC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBCBCBC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2192,247 +2893,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2898,7 +3358,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3610,11 +4070,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}" name="Summary" displayName="Summary" ref="A1:B4" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83" totalsRowBorderDxfId="82">
-  <autoFilter ref="A1:B4" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}" name="Summary" displayName="Summary" ref="A1:B5" totalsRowShown="0" headerRowDxfId="97" headerRowBorderDxfId="96" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+  <autoFilter ref="A1:B5" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{654C6343-7B3C-42FE-9EF4-7BFE7BE35779}" name="Test Case Sheet name" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{FDA0E746-B4F2-405E-8A1D-9A6A22073CB9}" name="Result" dataDxfId="80">
+    <tableColumn id="1" xr3:uid="{654C6343-7B3C-42FE-9EF4-7BFE7BE35779}" name="Test Case Sheet name" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{FDA0E746-B4F2-405E-8A1D-9A6A22073CB9}" name="Result" dataDxfId="92">
       <calculatedColumnFormula array="1">INDIRECT(A2&amp;"!E8")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3623,21 +4083,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}" name="SummaryResults" displayName="SummaryResults" ref="D1:E4" totalsRowShown="0" headerRowDxfId="79" headerRowBorderDxfId="78" tableBorderDxfId="77" totalsRowBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}" name="SummaryResults" displayName="SummaryResults" ref="D1:E4" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="D1:E4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5420B28C-70A3-47FD-BF8A-F016E4F7FA0F}" name="Summary Results" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{B0E66881-1E02-43BC-AA03-3C33769D1162}" name="Count" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{5420B28C-70A3-47FD-BF8A-F016E4F7FA0F}" name="Summary Results" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{B0E66881-1E02-43BC-AA03-3C33769D1162}" name="Count" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C89B2B93-96BB-441E-B77B-7E40B50E056D}" name="SampleTestCase12" displayName="SampleTestCase12" ref="A10:F35" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C89B2B93-96BB-441E-B77B-7E40B50E056D}" name="SampleTestCase12" displayName="SampleTestCase12" ref="A10:F35" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="81">
   <autoFilter ref="A10:F35" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3647,21 +4107,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{07F3C726-CF4B-4A89-9D4E-FFC2F3B71504}" name="Step#" dataDxfId="50">
+    <tableColumn id="1" xr3:uid="{07F3C726-CF4B-4A89-9D4E-FFC2F3B71504}" name="Step#" dataDxfId="80">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3B181203-88B8-4ECA-8586-E1A7969EA7C0}" name="Area" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{302EA2CC-144C-447A-9537-518BDA10AB76}" name="Step Details" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{9F997859-00F8-4561-BA64-59F450F04E06}" name="Expected" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{CAFD8264-06FC-4330-A577-54F901209313}" name="Actual" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{16774486-6CCF-4804-BFB8-5A09A9868319}" name="Status" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{3B181203-88B8-4ECA-8586-E1A7969EA7C0}" name="Area" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{302EA2CC-144C-447A-9537-518BDA10AB76}" name="Step Details" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{9F997859-00F8-4561-BA64-59F450F04E06}" name="Expected" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{CAFD8264-06FC-4330-A577-54F901209313}" name="Actual" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{16774486-6CCF-4804-BFB8-5A09A9868319}" name="Status" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3B579B8E-71E0-43F3-BD7B-444793913C5A}" name="SampleTestCase123" displayName="SampleTestCase123" ref="A10:F21" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3B579B8E-71E0-43F3-BD7B-444793913C5A}" name="SampleTestCase123" displayName="SampleTestCase123" ref="A10:F21" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71" totalsRowBorderDxfId="70">
   <autoFilter ref="A10:F21" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3671,21 +4131,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0AA68334-D062-478E-B0C8-2A2CFFD191F2}" name="Step#" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{0AA68334-D062-478E-B0C8-2A2CFFD191F2}" name="Step#" dataDxfId="69">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6AA83282-0CB1-43FB-B377-DD7C842943BA}" name="Area" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{1BC430D2-4E88-4EB3-A940-5C76D8B44147}" name="Step Details" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{A9EC0C70-AC5B-4C7B-9581-F62CC5CABAE0}" name="Expected" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{65718CE7-73C9-43E5-BEB5-4042B4E01F30}" name="Actual" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{F0DA7687-947E-491E-B21A-6C6F2A460B02}" name="Status" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{6AA83282-0CB1-43FB-B377-DD7C842943BA}" name="Area" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{1BC430D2-4E88-4EB3-A940-5C76D8B44147}" name="Step Details" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{A9EC0C70-AC5B-4C7B-9581-F62CC5CABAE0}" name="Expected" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{65718CE7-73C9-43E5-BEB5-4042B4E01F30}" name="Actual" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{F0DA7687-947E-491E-B21A-6C6F2A460B02}" name="Status" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2E377BD4-3235-49A1-8093-E3126E000F02}" name="SampleTestCase1236" displayName="SampleTestCase1236" ref="A10:F39" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2E377BD4-3235-49A1-8093-E3126E000F02}" name="SampleTestCase1236" displayName="SampleTestCase1236" ref="A10:F39" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="A10:F39" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3695,14 +4155,38 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D212E0A2-335D-478C-B756-642813E0558C}" name="Step#" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{D212E0A2-335D-478C-B756-642813E0558C}" name="Step#" dataDxfId="58">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16DCD7B5-32CF-48ED-AED3-35BA513DBB2D}" name="Area" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{AEE0C5E2-2C55-481B-8027-6186153E70AE}" name="Step Details" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{282D8BD2-B088-4502-A54F-900ED78CEE98}" name="Expected" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{EFCD6DDD-E11D-47C7-B40B-FC360F320FD4}" name="Actual" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{50EF06F8-03DD-4928-922F-2B85123D772A}" name="Status" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{16DCD7B5-32CF-48ED-AED3-35BA513DBB2D}" name="Area" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{AEE0C5E2-2C55-481B-8027-6186153E70AE}" name="Step Details" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{282D8BD2-B088-4502-A54F-900ED78CEE98}" name="Expected" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{EFCD6DDD-E11D-47C7-B40B-FC360F320FD4}" name="Actual" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{50EF06F8-03DD-4928-922F-2B85123D772A}" name="Status" dataDxfId="53"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7181037D-EAA8-477B-926D-5945EE5D476B}" name="SampleTestCase12367" displayName="SampleTestCase12367" ref="A10:F28" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49" totalsRowBorderDxfId="48">
+  <autoFilter ref="A10:F28" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C9D2A8EB-8A26-4DA3-B5C4-F1585D2B4AD3}" name="Step#" dataDxfId="47">
+      <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{E960D465-E197-49F4-A7D8-FAA1E145DCDA}" name="Area" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{EFD07A68-CBCE-4430-ADC4-005761F64FEE}" name="Step Details" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{42424136-EFC1-4D21-9325-71249B9AA2E2}" name="Expected" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{6F3A1C42-D6F8-4EAF-A3D2-A73A00CF2A1B}" name="Actual" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{054F85BC-5677-4522-B9A6-DF83175D1D72}" name="Status" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3971,10 +4455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1510635-E20C-4AD1-9756-3BB17945F573}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4013,7 +4497,7 @@
       </c>
       <c r="E2" s="5">
         <f ca="1">COUNTIF(Summary[Result],"Not Executed")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -4046,6 +4530,15 @@
       <c r="E4" s="9">
         <f ca="1">COUNTIF(Summary[Result],"Fail")</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="9" t="str" cm="1">
+        <f t="array" aca="1" ref="B5" ca="1">INDIRECT(A5&amp;"!E8")</f>
+        <v>Not Executed</v>
       </c>
     </row>
   </sheetData>
@@ -4065,7 +4558,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4087,14 +4580,14 @@
       <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4111,8 +4604,8 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
@@ -4127,8 +4620,8 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -4143,8 +4636,8 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
@@ -4159,17 +4652,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="28" t="str">
+      <c r="E8" s="26" t="str">
         <f>IF(E7&gt;0, "Fail",
     IF(E5&gt;0, "Not Executed", "Pass"))</f>
         <v>Not Executed</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -4198,7 +4691,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>20</v>
@@ -4208,7 +4701,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4217,7 +4710,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>38</v>
@@ -4227,7 +4720,7 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4236,7 +4729,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>136</v>
@@ -4246,48 +4739,48 @@
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="91" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>137</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" s="10"/>
+        <v>159</v>
+      </c>
+      <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="91" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>138</v>
+        <v>97</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E15" s="17"/>
+        <v>23</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="65" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4296,33 +4789,33 @@
         <v>97</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="65" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>37</v>
+        <v>98</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="E17" s="17"/>
       <c r="F17" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4334,14 +4827,14 @@
         <v>98</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4353,14 +4846,14 @@
         <v>98</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4372,14 +4865,14 @@
         <v>98</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4391,14 +4884,14 @@
         <v>98</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4410,14 +4903,14 @@
         <v>98</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4429,17 +4922,17 @@
         <v>98</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4448,17 +4941,17 @@
         <v>98</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -4467,14 +4960,14 @@
         <v>98</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>41</v>
+        <v>139</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4485,15 +4978,15 @@
       <c r="B26" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>142</v>
+      <c r="C26" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4504,15 +4997,15 @@
       <c r="B27" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>143</v>
+      <c r="C27" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4523,18 +5016,18 @@
       <c r="B28" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>144</v>
+      <c r="C28" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>29</v>
+        <v>148</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -4542,18 +5035,18 @@
       <c r="B29" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>145</v>
+      <c r="C29" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -4561,15 +5054,15 @@
       <c r="B30" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>146</v>
+      <c r="C30" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4580,78 +5073,78 @@
       <c r="B31" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>147</v>
+      <c r="C31" s="18" t="s">
+        <v>160</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f>IF(ISNUMBER(A30), A30 +1, 1)</f>
+        <v>21</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>148</v>
+      <c r="C32" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>149</v>
+      <c r="C33" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>150</v>
+      <c r="C34" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>99</v>
@@ -4664,7 +5157,7 @@
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4676,90 +5169,95 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F35">
-    <cfRule type="expression" dxfId="73" priority="3">
-      <formula>$F11="Fail"</formula>
+  <conditionalFormatting sqref="A11:E11 B12:E13 B15:E24 B25:B31 B33:C33 A12:A31 C25:E25 C26:C31 A33:A35">
+    <cfRule type="expression" dxfId="41" priority="8">
+      <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="4">
-      <formula>$F11="Pass"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B13 B15:B31 B33">
+    <cfRule type="expression" dxfId="40" priority="7">
+      <formula>AND($B11&lt;&gt;$B10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" dxfId="39" priority="62">
+      <formula>AND($B14&lt;&gt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32 B34">
+    <cfRule type="expression" dxfId="38" priority="54">
+      <formula>AND($B32&lt;&gt;$B30)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="37" priority="22">
+      <formula>AND($B35&lt;&gt;$B24)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:E14">
+    <cfRule type="expression" dxfId="36" priority="56">
+      <formula>AND($B14&lt;&gt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:E35">
+    <cfRule type="expression" dxfId="35" priority="20">
+      <formula>AND($B35&lt;&gt;$B24)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D31">
+    <cfRule type="expression" dxfId="34" priority="1">
+      <formula>AND($B26&lt;&gt;$B25)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:E33">
+    <cfRule type="expression" dxfId="33" priority="75">
+      <formula>AND($B32&lt;&gt;$B24)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:E34">
+    <cfRule type="expression" dxfId="32" priority="24">
+      <formula>AND($B34&lt;&gt;$B24)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="71" priority="5">
+    <cfRule type="expression" dxfId="31" priority="5">
       <formula>$E$8="Pass"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="6">
+    <cfRule type="expression" dxfId="30" priority="6">
       <formula>$E$8="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:E11 B26:B33 C27:C33 B12:E25 A12:A35 C26:E26">
-    <cfRule type="expression" dxfId="69" priority="8">
-      <formula>AND($B11&lt;&gt;$B10)</formula>
+  <conditionalFormatting sqref="E26 A32:C32 B34:C34">
+    <cfRule type="expression" dxfId="29" priority="48">
+      <formula>AND($B26&lt;&gt;$B24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B33">
-    <cfRule type="expression" dxfId="68" priority="7">
-      <formula>AND($B11&lt;&gt;$B10)</formula>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="expression" dxfId="28" priority="44">
+      <formula>AND($B27&lt;&gt;$B24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:E35">
-    <cfRule type="expression" dxfId="67" priority="20">
-      <formula>AND($B35&lt;&gt;$B25)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="66" priority="22">
-      <formula>AND($B35&lt;&gt;$B25)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34:E34">
-    <cfRule type="expression" dxfId="65" priority="24">
-      <formula>AND($B34&lt;&gt;$B25)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32:E33">
-    <cfRule type="expression" dxfId="64" priority="28">
-      <formula>AND($B32&lt;&gt;$B25)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" dxfId="63" priority="32">
-      <formula>AND($B31&lt;&gt;$B25)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
-    <cfRule type="expression" dxfId="62" priority="36">
-      <formula>AND($B30&lt;&gt;$B25)</formula>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="expression" dxfId="27" priority="40">
+      <formula>AND($B28&lt;&gt;$B24)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="61" priority="40">
-      <formula>AND($B29&lt;&gt;$B25)</formula>
+    <cfRule type="expression" dxfId="26" priority="36">
+      <formula>AND($B29&lt;&gt;$B24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="60" priority="44">
-      <formula>AND($B28&lt;&gt;$B25)</formula>
+  <conditionalFormatting sqref="E30:E31">
+    <cfRule type="expression" dxfId="25" priority="32">
+      <formula>AND($B30&lt;&gt;$B24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27 B34:C34">
-    <cfRule type="expression" dxfId="59" priority="48">
-      <formula>AND($B27&lt;&gt;$B25)</formula>
+  <conditionalFormatting sqref="F11:F35">
+    <cfRule type="expression" dxfId="24" priority="3">
+      <formula>$F11="Fail"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="58" priority="54">
-      <formula>AND($B34&lt;&gt;$B32)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:D28">
-    <cfRule type="expression" dxfId="57" priority="2">
-      <formula>AND($B27&lt;&gt;$B26)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D31">
-    <cfRule type="expression" dxfId="56" priority="1">
-      <formula>AND($B29&lt;&gt;$B28)</formula>
+    <cfRule type="expression" dxfId="23" priority="4">
+      <formula>$F11="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4779,7 +5277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EC76D5-508E-49A8-8CA4-8BD5DC983C38}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11:F21"/>
     </sheetView>
   </sheetViews>
@@ -4802,14 +5300,14 @@
       <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -4826,8 +5324,8 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
@@ -4842,8 +5340,8 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -4858,8 +5356,8 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
@@ -4874,17 +5372,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="28" t="str">
+      <c r="E8" s="26" t="str">
         <f>IF(E7&gt;0, "Fail",
     IF(E5&gt;0, "Not Executed", "Pass"))</f>
         <v>Not Executed</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -4923,7 +5421,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4935,14 +5433,14 @@
         <v>100</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4954,14 +5452,14 @@
         <v>100</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4980,7 +5478,7 @@
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4999,7 +5497,7 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5018,7 +5516,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5037,7 +5535,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5056,7 +5554,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5075,7 +5573,7 @@
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5094,7 +5592,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5113,7 +5611,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -5125,30 +5623,30 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F21">
-    <cfRule type="expression" dxfId="11" priority="1">
-      <formula>$F11="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
-      <formula>$F11="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>$E$8="Pass"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>$E$8="Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A11:E21">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B21">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>AND($B11&lt;&gt;$B10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="expression" dxfId="20" priority="3">
+      <formula>$E$8="Pass"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="4">
+      <formula>$E$8="Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F21">
+    <cfRule type="expression" dxfId="18" priority="1">
+      <formula>$F11="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="2">
+      <formula>$F11="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5168,8 +5666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0284662-B42C-4A0F-B1ED-3CE18BC81596}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5191,14 +5689,14 @@
       <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -5217,10 +5715,10 @@
       <c r="A5" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
@@ -5237,10 +5735,10 @@
       <c r="A6" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -5257,10 +5755,10 @@
       <c r="A7" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
@@ -5277,19 +5775,19 @@
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="28" t="str">
+      <c r="E8" s="26" t="str">
         <f>IF(E7&gt;0, "Fail",
     IF(E5&gt;0, "Not Executed", "Pass"))</f>
         <v>Not Executed</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -5328,7 +5826,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5340,14 +5838,14 @@
         <v>104</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5366,7 +5864,7 @@
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5385,7 +5883,7 @@
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5404,7 +5902,7 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5423,7 +5921,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5442,7 +5940,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5451,7 +5949,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>69</v>
@@ -5461,7 +5959,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5470,7 +5968,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>72</v>
@@ -5480,7 +5978,7 @@
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5489,7 +5987,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>73</v>
@@ -5499,7 +5997,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5508,7 +6006,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>91</v>
@@ -5518,7 +6016,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -5527,7 +6025,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>76</v>
@@ -5537,7 +6035,7 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5546,7 +6044,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>68</v>
@@ -5556,7 +6054,7 @@
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5575,7 +6073,7 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5594,7 +6092,7 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5613,7 +6111,7 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5632,7 +6130,7 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5651,7 +6149,7 @@
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5670,7 +6168,7 @@
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5689,7 +6187,7 @@
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5700,15 +6198,15 @@
       <c r="B31" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="23"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5719,7 +6217,7 @@
       <c r="B32" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="18" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -5727,7 +6225,7 @@
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5738,7 +6236,7 @@
       <c r="B33" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>121</v>
       </c>
       <c r="D33" s="10" t="s">
@@ -5746,7 +6244,7 @@
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5757,15 +6255,15 @@
       <c r="B34" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E34" s="23"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5776,15 +6274,15 @@
       <c r="B35" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5795,15 +6293,15 @@
       <c r="B36" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="23"/>
+      <c r="E36" s="21"/>
       <c r="F36" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5814,15 +6312,15 @@
       <c r="B37" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="21"/>
       <c r="F37" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5833,15 +6331,15 @@
       <c r="B38" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="21"/>
       <c r="F38" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5852,15 +6350,15 @@
       <c r="B39" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E39" s="23"/>
+      <c r="E39" s="21"/>
       <c r="F39" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -5872,55 +6370,55 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F39">
-    <cfRule type="expression" dxfId="33" priority="5">
-      <formula>$F11="Fail"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="6">
-      <formula>$F11="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="31" priority="7">
-      <formula>$E$8="Pass"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="8">
-      <formula>$E$8="Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11:F11 C32:F32 B31:B35 B37:B39 B36:F36 A12:A39 B12:F31 F12:F39">
-    <cfRule type="expression" dxfId="29" priority="10">
+  <conditionalFormatting sqref="A11:F11 B12:F31 B31:B35 B36:F36 B37:B39 F12:F39 C32:F32 A12:A39">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B39">
-    <cfRule type="expression" dxfId="28" priority="9">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:F33">
-    <cfRule type="expression" dxfId="27" priority="16">
-      <formula>AND($B33&lt;&gt;#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C34:D34">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>AND($B34&lt;&gt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:D35">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>AND($B35&lt;&gt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F37:F39">
-    <cfRule type="expression" dxfId="24" priority="2">
-      <formula>AND($B37&lt;&gt;$B36)</formula>
+  <conditionalFormatting sqref="C33:F33">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>AND($B33&lt;&gt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>AND($B38&lt;&gt;$B37)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="expression" dxfId="10" priority="7">
+      <formula>$E$8="Pass"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="8">
+      <formula>$E$8="Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F39">
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>$F11="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="6">
+      <formula>$F11="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37:F39">
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>AND($B37&lt;&gt;$B36)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5934,4 +6432,530 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753BFD3A-0EAD-4FCE-88E1-476450540439}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" customWidth="1"/>
+    <col min="3" max="5" width="38.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5">
+        <f>COUNTIF(SampleTestCase12367[Status], "Not Executed")</f>
+        <v>18</v>
+      </c>
+      <c r="F5" s="15">
+        <f>E5/SUM(E$5:E$7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="16"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5">
+        <f>COUNTIF(SampleTestCase12367[Status], "Pass")</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="15">
+        <f t="shared" ref="F6:F7" si="0">E6/SUM(E$5:E$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="16"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5">
+        <f>COUNTIF(SampleTestCase12367[Status], "Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="16"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="26" t="str">
+        <f>IF(E7&gt;0, "Fail",
+    IF(E5&gt;0, "Not Executed", "Pass"))</f>
+        <v>Not Executed</v>
+      </c>
+      <c r="F8" s="26"/>
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <f t="shared" ref="A11:A28" si="1">IF(ISNUMBER(A10), A10 +1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="91" x14ac:dyDescent="0.35">
+      <c r="A20" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A22" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="5">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:F8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A11:F28">
+    <cfRule type="expression" dxfId="5" priority="10">
+      <formula>AND($B11&lt;&gt;$B10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B28">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>AND($B11&lt;&gt;$B10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>$E$8="Pass"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>$E$8="Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F28">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$F11="Fail"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>$F11="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F28" xr:uid="{0FFC8341-0802-409B-B910-7C3C2697A542}">
+      <formula1>"Pass,Fail,Not Executed"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Regression test execution of 20240320_001
</commit_message>
<xml_diff>
--- a/doc/regression-test/suites/legacy-security/01-basic.xlsx
+++ b/doc/regression-test/suites/legacy-security/01-basic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\Dev\Propel\propel\doc\regression-test\suites\legacy-security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912F5483-C330-4E9B-8D6F-D6DF96F19684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DB1750-8BB3-40B4-B522-013F73621F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="209">
   <si>
     <t>Description</t>
   </si>
@@ -363,9 +363,6 @@
   <si>
     <t>Home Page is displayed.
 The blue user icon from Legacy security is displayed in the top right corner</t>
-  </si>
-  <si>
-    <t>When ypou click the Save button in the Finish tab you will see an error toast saying "The item already exists!"</t>
   </si>
   <si>
     <t>Change the field Script name from the value "Test Remote" to "Test Remote 2"</t>
@@ -731,6 +728,17 @@
   <si>
     <t>You will see a toast indicating the changes have been saved successfully.
 Also, "cancel" button is now disabled.</t>
+  </si>
+  <si>
+    <t>When you click the Save button in the Finish tab you will see an error toast saying "The item already exists!"</t>
+  </si>
+  <si>
+    <t>A toast indicates the changes have been saved successfully.
+All tabs are now disabled.
+A new "Add another" script button is now present.</t>
+  </si>
+  <si>
+    <t>Click the "Save" button.</t>
   </si>
 </sst>
 </file>
@@ -4502,7 +4510,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">INDIRECT(A3&amp;"!E8")</f>
@@ -4518,7 +4526,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B4" ca="1">INDIRECT(A4&amp;"!E8")</f>
@@ -4534,7 +4542,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="9" t="str" cm="1">
         <f t="array" aca="1" ref="B5" ca="1">INDIRECT(A5&amp;"!E8")</f>
@@ -4557,8 +4565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59558529-F109-4122-99C6-22F7311C314B}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4670,7 +4678,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>6</v>
@@ -4691,7 +4699,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>20</v>
@@ -4701,7 +4709,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4710,7 +4718,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>38</v>
@@ -4720,7 +4728,7 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4729,17 +4737,17 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="91" x14ac:dyDescent="0.35">
@@ -4748,17 +4756,17 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4767,7 +4775,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>36</v>
@@ -4777,7 +4785,7 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -4786,17 +4794,17 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4805,7 +4813,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>34</v>
@@ -4815,7 +4823,7 @@
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4824,7 +4832,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>24</v>
@@ -4834,7 +4842,7 @@
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4843,7 +4851,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>26</v>
@@ -4853,7 +4861,7 @@
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4862,7 +4870,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>28</v>
@@ -4872,7 +4880,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4881,7 +4889,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>30</v>
@@ -4891,7 +4899,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4900,7 +4908,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>32</v>
@@ -4910,7 +4918,7 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4919,7 +4927,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>40</v>
@@ -4929,7 +4937,7 @@
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -4938,7 +4946,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>41</v>
@@ -4948,7 +4956,7 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4957,17 +4965,17 @@
         <v>15</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>35</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4976,17 +4984,17 @@
         <v>16</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4995,17 +5003,17 @@
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5014,17 +5022,17 @@
         <v>18</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5033,17 +5041,17 @@
         <v>19</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5052,17 +5060,17 @@
         <v>20</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5071,17 +5079,17 @@
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>160</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>161</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5090,17 +5098,17 @@
         <v>21</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5109,17 +5117,17 @@
         <v>22</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5128,17 +5136,17 @@
         <v>23</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5147,7 +5155,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>45</v>
@@ -5157,7 +5165,7 @@
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -5277,7 +5285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EC76D5-508E-49A8-8CA4-8BD5DC983C38}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="F11" sqref="F11:F21"/>
     </sheetView>
   </sheetViews>
@@ -5390,7 +5398,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>6</v>
@@ -5411,7 +5419,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>20</v>
@@ -5421,7 +5429,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5430,17 +5438,17 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5449,17 +5457,17 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5468,7 +5476,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>60</v>
@@ -5478,7 +5486,7 @@
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5487,7 +5495,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>49</v>
@@ -5497,7 +5505,7 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5506,7 +5514,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>51</v>
@@ -5516,7 +5524,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5525,7 +5533,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>62</v>
@@ -5535,7 +5543,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5544,7 +5552,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>54</v>
@@ -5554,7 +5562,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5563,7 +5571,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>55</v>
@@ -5573,7 +5581,7 @@
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5582,7 +5590,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>58</v>
@@ -5592,7 +5600,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5601,7 +5609,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>55</v>
@@ -5611,7 +5619,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -5666,8 +5674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0284662-B42C-4A0F-B1ED-3CE18BC81596}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5690,7 +5698,7 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -5713,10 +5721,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
@@ -5733,10 +5741,10 @@
     </row>
     <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>115</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>116</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="1" t="s">
@@ -5753,10 +5761,10 @@
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="1" t="s">
@@ -5773,10 +5781,10 @@
     </row>
     <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="6" t="s">
@@ -5795,7 +5803,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>6</v>
@@ -5816,7 +5824,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>20</v>
@@ -5826,7 +5834,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5835,17 +5843,17 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5854,17 +5862,17 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5873,7 +5881,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>64</v>
@@ -5883,7 +5891,7 @@
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5892,17 +5900,17 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5911,7 +5919,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>64</v>
@@ -5921,7 +5929,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5930,7 +5938,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>68</v>
@@ -5940,7 +5948,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5949,7 +5957,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>69</v>
@@ -5959,7 +5967,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5968,17 +5976,17 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>72</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>90</v>
+        <v>206</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5987,7 +5995,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>73</v>
@@ -5997,7 +6005,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6006,17 +6014,17 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -6025,7 +6033,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>76</v>
@@ -6035,7 +6043,7 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -6044,17 +6052,17 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>68</v>
+        <v>208</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>70</v>
+        <v>207</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6063,7 +6071,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>78</v>
@@ -6073,7 +6081,7 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6082,7 +6090,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>79</v>
@@ -6092,7 +6100,7 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6101,7 +6109,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>81</v>
@@ -6111,7 +6119,7 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6120,7 +6128,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>84</v>
@@ -6130,7 +6138,7 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6139,7 +6147,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>86</v>
@@ -6149,7 +6157,7 @@
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6158,7 +6166,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>88</v>
@@ -6168,7 +6176,7 @@
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6177,7 +6185,7 @@
         <v>20</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>86</v>
@@ -6187,7 +6195,7 @@
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6196,17 +6204,17 @@
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6215,17 +6223,17 @@
         <v>22</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6234,17 +6242,17 @@
         <v>23</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6253,17 +6261,17 @@
         <v>24</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C34" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="20" t="s">
         <v>123</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>124</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6272,17 +6280,17 @@
         <v>25</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C35" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>126</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6291,17 +6299,17 @@
         <v>26</v>
       </c>
       <c r="B36" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="D36" s="20" t="s">
         <v>128</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>129</v>
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6310,17 +6318,17 @@
         <v>27</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C37" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>131</v>
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6329,17 +6337,17 @@
         <v>28</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6348,17 +6356,17 @@
         <v>29</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>133</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>134</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -6438,7 +6446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753BFD3A-0EAD-4FCE-88E1-476450540439}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -6462,7 +6470,7 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -6485,10 +6493,10 @@
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
@@ -6555,7 +6563,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>6</v>
@@ -6576,7 +6584,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>20</v>
@@ -6586,7 +6594,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6595,17 +6603,17 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>204</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>205</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6614,17 +6622,17 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6633,17 +6641,17 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6652,17 +6660,17 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>175</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>176</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6671,17 +6679,17 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6690,17 +6698,17 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6709,17 +6717,17 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>179</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>180</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6728,17 +6736,17 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="91" x14ac:dyDescent="0.35">
@@ -6747,17 +6755,17 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>182</v>
-      </c>
       <c r="D20" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6766,17 +6774,17 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C21" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>186</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6785,17 +6793,17 @@
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6804,17 +6812,17 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="D23" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6823,17 +6831,17 @@
         <v>14</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6842,17 +6850,17 @@
         <v>15</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="D25" s="10" t="s">
         <v>195</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>196</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -6861,17 +6869,17 @@
         <v>16</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="D26" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>199</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6880,17 +6888,17 @@
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6899,17 +6907,17 @@
         <v>18</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C28" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>202</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>